<commit_message>
Added dbscan, changed output
</commit_message>
<xml_diff>
--- a/outputs/clustered_examples.xlsx
+++ b/outputs/clustered_examples.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F88"/>
+  <dimension ref="A1:E88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,15 +451,10 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Smiles</t>
+          <t>km_cluster</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>km_cluster</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>db_cluster</t>
         </is>
@@ -477,15 +472,10 @@
       <c r="C2" t="n">
         <v>1</v>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>CN1CC[C@]23c4c5ccc(O)c4O[C@H]2[C@@H](O)C=C[C@H]3[C@H]1C5</t>
-        </is>
+      <c r="D2" t="n">
+        <v>1</v>
       </c>
       <c r="E2" t="n">
-        <v>1</v>
-      </c>
-      <c r="F2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -501,15 +491,10 @@
       <c r="C3" t="n">
         <v>1</v>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>COc1ccc2c3c1O[C@H]1[C@@H](O)C=C[C@H]4[C@@H](C2)N(C)CC[C@@]341</t>
-        </is>
+      <c r="D3" t="n">
+        <v>1</v>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
-      </c>
-      <c r="F3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -525,15 +510,10 @@
       <c r="C4" t="n">
         <v>0</v>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>COc1ccc2c(c1OC)C(=O)O[C@@H]2[C@H]1c2c(cc3c(c2OC)OCO3)CCN1C</t>
-        </is>
+      <c r="D4" t="n">
+        <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
-      </c>
-      <c r="F4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -549,16 +529,11 @@
       <c r="C5" t="n">
         <v>0</v>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>COc1ccc(Cc2nccc3cc(OC)c(OC)cc23)cc1OC</t>
-        </is>
+      <c r="D5" t="n">
+        <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -573,15 +548,10 @@
       <c r="C6" t="n">
         <v>0</v>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>CC(=O)Oc1ccc2c3c1O[C@H]1[C@@H](OC(C)=O)C=C[C@H]4[C@@H](C2)N(C)CC[C@@]341</t>
-        </is>
+      <c r="D6" t="n">
+        <v>1</v>
       </c>
       <c r="E6" t="n">
-        <v>1</v>
-      </c>
-      <c r="F6" t="n">
         <v>0</v>
       </c>
     </row>
@@ -597,15 +567,10 @@
       <c r="C7" t="n">
         <v>1</v>
       </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>COc1ccc2c3c1O[C@H]1C(=O)CC[C@@]4(O)[C@@H](C2)N(C)CC[C@]314</t>
-        </is>
+      <c r="D7" t="n">
+        <v>1</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -621,15 +586,10 @@
       <c r="C8" t="n">
         <v>0</v>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>CCOc1ccc2c3c1O[C@H]1[C@@H](O)C=C[C@H]4[C@@H](C2)N(C)CC[C@@]341</t>
-        </is>
+      <c r="D8" t="n">
+        <v>1</v>
       </c>
       <c r="E8" t="n">
-        <v>1</v>
-      </c>
-      <c r="F8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -645,16 +605,11 @@
       <c r="C9" t="n">
         <v>1</v>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>CCC(=O)C(CC(C)N(C)C)(c1ccccc1)c1ccccc1</t>
-        </is>
+      <c r="D9" t="n">
+        <v>0</v>
       </c>
       <c r="E9" t="n">
         <v>1</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -669,15 +624,10 @@
       <c r="C10" t="n">
         <v>1</v>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>COc1ccc2c3c1O[C@H]1[C@@H](O)CC[C@H]4[C@@H](C2)N(C)CC[C@@]341</t>
-        </is>
+      <c r="D10" t="n">
+        <v>1</v>
       </c>
       <c r="E10" t="n">
-        <v>1</v>
-      </c>
-      <c r="F10" t="n">
         <v>0</v>
       </c>
     </row>
@@ -693,15 +643,10 @@
       <c r="C11" t="n">
         <v>1</v>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>COc1cccc(C2(O)CCCCC2CN(C)C)c1</t>
-        </is>
+      <c r="D11" t="n">
+        <v>1</v>
       </c>
       <c r="E11" t="n">
-        <v>0</v>
-      </c>
-      <c r="F11" t="n">
         <v>0</v>
       </c>
     </row>
@@ -717,15 +662,10 @@
       <c r="C12" t="n">
         <v>0</v>
       </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>CC(C)=CCN1CCC2(C)c3cc(O)ccc3CC1C2C</t>
-        </is>
+      <c r="D12" t="n">
+        <v>1</v>
       </c>
       <c r="E12" t="n">
-        <v>1</v>
-      </c>
-      <c r="F12" t="n">
         <v>0</v>
       </c>
     </row>
@@ -741,15 +681,10 @@
       <c r="C13" t="n">
         <v>1</v>
       </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>Oc1ccc2c(c1)[C@@]13CCCC[C@@]1(O)[C@@H](C2)N(CC1CCC1)CC3</t>
-        </is>
+      <c r="D13" t="n">
+        <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>1</v>
-      </c>
-      <c r="F13" t="n">
         <v>0</v>
       </c>
     </row>
@@ -765,15 +700,10 @@
       <c r="C14" t="n">
         <v>1</v>
       </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>Oc1ccc2c3c1O[C@H]1[C@@H](O)CC[C@@]4(O)[C@@H](C2)N(CC2CCC2)CC[C@]314</t>
-        </is>
+      <c r="D14" t="n">
+        <v>0</v>
       </c>
       <c r="E14" t="n">
-        <v>0</v>
-      </c>
-      <c r="F14" t="n">
         <v>0</v>
       </c>
     </row>
@@ -789,15 +719,10 @@
       <c r="C15" t="n">
         <v>1</v>
       </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>CN1CC[C@]23CCCC[C@H]2[C@H]1Cc1ccc(O)cc13</t>
-        </is>
+      <c r="D15" t="n">
+        <v>1</v>
       </c>
       <c r="E15" t="n">
-        <v>1</v>
-      </c>
-      <c r="F15" t="n">
         <v>0</v>
       </c>
     </row>
@@ -813,16 +738,11 @@
       <c r="C16" t="n">
         <v>0</v>
       </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>CC[C@@H](c1cccc(O)c1)[C@@H](C)CN(C)C</t>
-        </is>
+      <c r="D16" t="n">
+        <v>0</v>
       </c>
       <c r="E16" t="n">
         <v>1</v>
-      </c>
-      <c r="F16" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -837,16 +757,11 @@
       <c r="C17" t="n">
         <v>1</v>
       </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>CCOC(=O)C1(c2ccccc2)CCN(C)CC1</t>
-        </is>
+      <c r="D17" t="n">
+        <v>1</v>
       </c>
       <c r="E17" t="n">
         <v>1</v>
-      </c>
-      <c r="F17" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -861,16 +776,11 @@
       <c r="C18" t="n">
         <v>1</v>
       </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>CCC(=O)N(c1ccccc1)C1CCN(CCc2ccccc2)CC1</t>
-        </is>
+      <c r="D18" t="n">
+        <v>1</v>
       </c>
       <c r="E18" t="n">
         <v>1</v>
-      </c>
-      <c r="F18" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -885,16 +795,11 @@
       <c r="C19" t="n">
         <v>1</v>
       </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>CCC(=O)N(c1ccccc1)C1(COC)CCN(CCc2cccs2)CC1</t>
-        </is>
+      <c r="D19" t="n">
+        <v>1</v>
       </c>
       <c r="E19" t="n">
         <v>1</v>
-      </c>
-      <c r="F19" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -909,16 +814,11 @@
       <c r="C20" t="n">
         <v>1</v>
       </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>CCC(=O)N(c1ccccc1)C1(COC)CCN(CCn2nnn(CC)c2=O)CC1</t>
-        </is>
+      <c r="D20" t="n">
+        <v>1</v>
       </c>
       <c r="E20" t="n">
         <v>1</v>
-      </c>
-      <c r="F20" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -933,16 +833,11 @@
       <c r="C21" t="n">
         <v>1</v>
       </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>CCC(=O)N(c1ccccc1)C1(C(=O)OC)CCN(CCC(=O)OC)CC1</t>
-        </is>
+      <c r="D21" t="n">
+        <v>1</v>
       </c>
       <c r="E21" t="n">
         <v>1</v>
-      </c>
-      <c r="F21" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -957,16 +852,11 @@
       <c r="C22" t="n">
         <v>0</v>
       </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>CN(C)C(=O)C(CCN1CCC(O)(c2ccc(Cl)cc2)CC1)(c1ccccc1)c1ccccc1</t>
-        </is>
+      <c r="D22" t="n">
+        <v>1</v>
       </c>
       <c r="E22" t="n">
         <v>1</v>
-      </c>
-      <c r="F22" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -981,15 +871,10 @@
       <c r="C23" t="n">
         <v>1</v>
       </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>CO[C@@]12CC[C@@]3(C[C@@H]1[C@](C)(O)C(C)(C)C)[C@H]1Cc4ccc(O)c5c4[C@@]3(CCN1CC1CC1)[C@H]2O5</t>
-        </is>
+      <c r="D23" t="n">
+        <v>1</v>
       </c>
       <c r="E23" t="n">
-        <v>0</v>
-      </c>
-      <c r="F23" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1005,15 +890,10 @@
       <c r="C24" t="n">
         <v>1</v>
       </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>CN1CC[C@]23c4c5ccc(O)c4O[C@H]2C(=O)CC[C@@]3(O)[C@H]1C5</t>
-        </is>
+      <c r="D24" t="n">
+        <v>1</v>
       </c>
       <c r="E24" t="n">
-        <v>0</v>
-      </c>
-      <c r="F24" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1029,15 +909,10 @@
       <c r="C25" t="n">
         <v>1</v>
       </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>CN1CC[C@]23c4c5ccc(O)c4O[C@H]2C(=O)CC[C@H]3[C@H]1C5</t>
-        </is>
+      <c r="D25" t="n">
+        <v>1</v>
       </c>
       <c r="E25" t="n">
-        <v>1</v>
-      </c>
-      <c r="F25" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1053,15 +928,10 @@
       <c r="C26" t="n">
         <v>0</v>
       </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>O=C1CC[C@@]2(O)[C@H]3Cc4ccc(O)c5c4[C@@]2(CCN3CC2CC2)[C@H]1O5</t>
-        </is>
+      <c r="D26" t="n">
+        <v>0</v>
       </c>
       <c r="E26" t="n">
-        <v>0</v>
-      </c>
-      <c r="F26" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1077,15 +947,10 @@
       <c r="C27" t="n">
         <v>0</v>
       </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>C=CCN1CC[C@]23c4c5ccc(O)c4O[C@H]2C(=O)CC[C@@]3(O)[C@H]1C5</t>
-        </is>
+      <c r="D27" t="n">
+        <v>1</v>
       </c>
       <c r="E27" t="n">
-        <v>0</v>
-      </c>
-      <c r="F27" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1101,16 +966,11 @@
       <c r="C28" t="n">
         <v>1</v>
       </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>CCC(=O)O[C@](Cc1ccccc1)(c1ccccc1)[C@H](C)CN(C)C</t>
-        </is>
+      <c r="D28" t="n">
+        <v>0</v>
       </c>
       <c r="E28" t="n">
         <v>1</v>
-      </c>
-      <c r="F28" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="29">
@@ -1125,16 +985,11 @@
       <c r="C29" t="n">
         <v>0</v>
       </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>CCOC(=O)C1(c2ccccc2)CCN(CCC(C#N)(c2ccccc2)c2ccccc2)CC1</t>
-        </is>
+      <c r="D29" t="n">
+        <v>1</v>
       </c>
       <c r="E29" t="n">
         <v>1</v>
-      </c>
-      <c r="F29" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="30">
@@ -1149,15 +1004,10 @@
       <c r="C30" t="n">
         <v>0</v>
       </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>CCC[C@@](C)(O)[C@H]1C[C@@]23C=C[C@]1(OC)[C@@H]1Oc4c(O)ccc5c4[C@@]12CCN(C)[C@@H]3C5</t>
-        </is>
+      <c r="D30" t="n">
+        <v>1</v>
       </c>
       <c r="E30" t="n">
-        <v>1</v>
-      </c>
-      <c r="F30" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1173,16 +1023,11 @@
       <c r="C31" t="n">
         <v>0</v>
       </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>CNC1(c2ccccc2Cl)CCCCC1=O</t>
-        </is>
+      <c r="D31" t="n">
+        <v>0</v>
       </c>
       <c r="E31" t="n">
         <v>1</v>
-      </c>
-      <c r="F31" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="32">
@@ -1197,15 +1042,10 @@
       <c r="C32" t="n">
         <v>0</v>
       </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>CC[C@@H]1CN2CCc3c([nH]c4cccc(OC)c34)[C@@H]2C[C@@H]1/C(=C\OC)C(=O)OC</t>
-        </is>
+      <c r="D32" t="n">
+        <v>1</v>
       </c>
       <c r="E32" t="n">
-        <v>1</v>
-      </c>
-      <c r="F32" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1221,15 +1061,10 @@
       <c r="C33" t="n">
         <v>0</v>
       </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>CO/C=C(/C(=O)OC)[C@@H]1CCN2CC[C@]3(Nc4cccc(OC)c4C3=O)[C@@H]2C1</t>
-        </is>
+      <c r="D33" t="n">
+        <v>1</v>
       </c>
       <c r="E33" t="n">
-        <v>0</v>
-      </c>
-      <c r="F33" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1245,15 +1080,10 @@
       <c r="C34" t="n">
         <v>0</v>
       </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>COC1=CC=C2[C@H]3Cc4ccc(OC)c5c4[C@@]2(CCN3C)[C@H]1O5</t>
-        </is>
+      <c r="D34" t="n">
+        <v>1</v>
       </c>
       <c r="E34" t="n">
-        <v>1</v>
-      </c>
-      <c r="F34" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1269,15 +1099,10 @@
       <c r="C35" t="n">
         <v>0</v>
       </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>CN1CCc2cccc3c2[C@H]1Cc1ccc(O)c(O)c1-3</t>
-        </is>
+      <c r="D35" t="n">
+        <v>1</v>
       </c>
       <c r="E35" t="n">
-        <v>1</v>
-      </c>
-      <c r="F35" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1293,15 +1118,10 @@
       <c r="C36" t="n">
         <v>0</v>
       </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>CCC[C@H](C)C1C[C@@]23C=C[C@]1(OC)[C@@H]1Oc4cccc5c4[C@@]12CCN(C)[C@@H]3C5</t>
-        </is>
+      <c r="D36" t="n">
+        <v>1</v>
       </c>
       <c r="E36" t="n">
-        <v>1</v>
-      </c>
-      <c r="F36" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1317,16 +1137,11 @@
       <c r="C37" t="n">
         <v>1</v>
       </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>CC(=O)Nc1ccc(O)cc1</t>
-        </is>
+      <c r="D37" t="n">
+        <v>0</v>
       </c>
       <c r="E37" t="n">
         <v>1</v>
-      </c>
-      <c r="F37" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="38">
@@ -1341,16 +1156,11 @@
       <c r="C38" t="n">
         <v>0</v>
       </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>CC(C)Cc1ccc(C(C)C(=O)O)cc1</t>
-        </is>
+      <c r="D38" t="n">
+        <v>0</v>
       </c>
       <c r="E38" t="n">
         <v>1</v>
-      </c>
-      <c r="F38" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="39">
@@ -1365,16 +1175,11 @@
       <c r="C39" t="n">
         <v>1</v>
       </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>CC(=O)Oc1ccccc1C(=O)O</t>
-        </is>
+      <c r="D39" t="n">
+        <v>0</v>
       </c>
       <c r="E39" t="n">
         <v>1</v>
-      </c>
-      <c r="F39" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="40">
@@ -1389,16 +1194,11 @@
       <c r="C40" t="n">
         <v>0</v>
       </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>CC(C)NCC(O)COc1ccc(CC(N)=O)cc1</t>
-        </is>
+      <c r="D40" t="n">
+        <v>0</v>
       </c>
       <c r="E40" t="n">
-        <v>0</v>
-      </c>
-      <c r="F40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41">
@@ -1413,16 +1213,11 @@
       <c r="C41" t="n">
         <v>0</v>
       </c>
-      <c r="D41" t="inlineStr">
-        <is>
-          <t>CN1C(=O)CN=C(c2ccccc2)c2cc(Cl)ccc21</t>
-        </is>
+      <c r="D41" t="n">
+        <v>0</v>
       </c>
       <c r="E41" t="n">
         <v>1</v>
-      </c>
-      <c r="F41" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="42">
@@ -1437,15 +1232,10 @@
       <c r="C42" t="n">
         <v>0</v>
       </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>CCC(C)(C)C(=O)O[C@H]1C[C@@H](C)C=C2C=C[C@H](C)[C@H](CC[C@@H]3C[C@@H](O)CC(=O)O3)[C@H]21</t>
-        </is>
+      <c r="D42" t="n">
+        <v>0</v>
       </c>
       <c r="E42" t="n">
-        <v>1</v>
-      </c>
-      <c r="F42" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1461,15 +1251,10 @@
       <c r="C43" t="n">
         <v>0</v>
       </c>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>CCCCc1oc2ccccc2c1C(=O)c1cc(I)c(OCCN(CC)CC)c(I)c1</t>
-        </is>
+      <c r="D43" t="n">
+        <v>0</v>
       </c>
       <c r="E43" t="n">
-        <v>0</v>
-      </c>
-      <c r="F43" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1485,15 +1270,10 @@
       <c r="C44" t="n">
         <v>0</v>
       </c>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t>CC[C@H]1OC(=O)[C@H](C)[C@@H](O[C@H]2C[C@@](C)(OC)[C@@H](O)[C@H](C)O2)[C@H](C)[C@@H](O[C@@H]2O[C@H](C)C[C@H](N(C)C)[C@H]2O)[C@](C)(O)C[C@@H](C)CN(C)[C@H](C)[C@@H](O)[C@]1(C)O</t>
-        </is>
+      <c r="D44" t="n">
+        <v>0</v>
       </c>
       <c r="E44" t="n">
-        <v>0</v>
-      </c>
-      <c r="F44" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1509,16 +1289,11 @@
       <c r="C45" t="n">
         <v>0</v>
       </c>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t>CC(=O)CC(c1ccccc1)c1c(O)c2ccccc2oc1=O</t>
-        </is>
+      <c r="D45" t="n">
+        <v>1</v>
       </c>
       <c r="E45" t="n">
         <v>1</v>
-      </c>
-      <c r="F45" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="46">
@@ -1533,16 +1308,11 @@
       <c r="C46" t="n">
         <v>0</v>
       </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>CN(C)C(=N)NC(=N)N</t>
-        </is>
+      <c r="D46" t="n">
+        <v>0</v>
       </c>
       <c r="E46" t="n">
         <v>1</v>
-      </c>
-      <c r="F46" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="47">
@@ -1557,15 +1327,10 @@
       <c r="C47" t="n">
         <v>0</v>
       </c>
-      <c r="D47" t="inlineStr">
-        <is>
-          <t>CCOC(=O)N1CCC(=C2c3ccc(Cl)cc3CCc3cccnc32)CC1</t>
-        </is>
+      <c r="D47" t="n">
+        <v>0</v>
       </c>
       <c r="E47" t="n">
-        <v>1</v>
-      </c>
-      <c r="F47" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1581,15 +1346,10 @@
       <c r="C48" t="n">
         <v>0</v>
       </c>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t>CC(C)c1c(C(=O)Nc2ccccc2)c(-c2ccccc2)c(-c2ccc(F)cc2)n1CC[C@@H](O)C[C@@H](O)CC(=O)O</t>
-        </is>
+      <c r="D48" t="n">
+        <v>0</v>
       </c>
       <c r="E48" t="n">
-        <v>0</v>
-      </c>
-      <c r="F48" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1605,15 +1365,10 @@
       <c r="C49" t="n">
         <v>0</v>
       </c>
-      <c r="D49" t="inlineStr">
-        <is>
-          <t>CNC(=C[N+](=O)[O-])NCCSCc1ccc(CN(C)C)o1</t>
-        </is>
+      <c r="D49" t="n">
+        <v>0</v>
       </c>
       <c r="E49" t="n">
-        <v>0</v>
-      </c>
-      <c r="F49" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1629,15 +1384,10 @@
       <c r="C50" t="n">
         <v>0</v>
       </c>
-      <c r="D50" t="inlineStr">
-        <is>
-          <t>NS(=O)(=O)c1cc(C(=O)O)c(NCc2ccco2)cc1Cl</t>
-        </is>
+      <c r="D50" t="n">
+        <v>0</v>
       </c>
       <c r="E50" t="n">
-        <v>1</v>
-      </c>
-      <c r="F50" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1653,15 +1403,10 @@
       <c r="C51" t="n">
         <v>0</v>
       </c>
-      <c r="D51" t="inlineStr">
-        <is>
-          <t>C[C@@H]1C[C@H]2[C@@H]3CCC4=CC(=O)C=C[C@]4(C)[C@@]3(F)[C@@H](O)C[C@]2(C)[C@@]1(O)C(=O)CO</t>
-        </is>
+      <c r="D51" t="n">
+        <v>0</v>
       </c>
       <c r="E51" t="n">
-        <v>0</v>
-      </c>
-      <c r="F51" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1677,16 +1422,11 @@
       <c r="C52" t="n">
         <v>0</v>
       </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>COc1ccc2[nH]c([S+]([O-])Cc3ncc(C)c(OC)c3C)nc2c1</t>
-        </is>
+      <c r="D52" t="n">
+        <v>0</v>
       </c>
       <c r="E52" t="n">
         <v>0</v>
-      </c>
-      <c r="F52" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="53">
@@ -1701,15 +1441,10 @@
       <c r="C53" t="n">
         <v>0</v>
       </c>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t>CCOC(=O)C1=C(COCCN)NC(C)=C(C(=O)OC)C1c1ccccc1Cl</t>
-        </is>
+      <c r="D53" t="n">
+        <v>0</v>
       </c>
       <c r="E53" t="n">
-        <v>0</v>
-      </c>
-      <c r="F53" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1725,15 +1460,10 @@
       <c r="C54" t="n">
         <v>0</v>
       </c>
-      <c r="D54" t="inlineStr">
-        <is>
-          <t>N[C@@H](Cc1cc(I)c(Oc2cc(I)c(O)c(I)c2)c(I)c1)C(=O)O</t>
-        </is>
+      <c r="D54" t="n">
+        <v>0</v>
       </c>
       <c r="E54" t="n">
-        <v>1</v>
-      </c>
-      <c r="F54" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1749,16 +1479,11 @@
       <c r="C55" t="n">
         <v>0</v>
       </c>
-      <c r="D55" t="inlineStr">
-        <is>
-          <t>O=C(O)c1cn(C2CC2)c2cc(N3CCNCC3)c(F)cc2c1=O</t>
-        </is>
+      <c r="D55" t="n">
+        <v>0</v>
       </c>
       <c r="E55" t="n">
         <v>1</v>
-      </c>
-      <c r="F55" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="56">
@@ -1773,15 +1498,10 @@
       <c r="C56" t="n">
         <v>0</v>
       </c>
-      <c r="D56" t="inlineStr">
-        <is>
-          <t>COc1ccc(Cl)cc1C(=O)NCCc1ccc(S(=O)(=O)NC(=O)NC2CCCCC2)cc1</t>
-        </is>
+      <c r="D56" t="n">
+        <v>0</v>
       </c>
       <c r="E56" t="n">
-        <v>0</v>
-      </c>
-      <c r="F56" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1797,16 +1517,11 @@
       <c r="C57" t="n">
         <v>0</v>
       </c>
-      <c r="D57" t="inlineStr">
-        <is>
-          <t>COCCc1ccc(OCC(O)CNC(C)C)cc1</t>
-        </is>
+      <c r="D57" t="n">
+        <v>0</v>
       </c>
       <c r="E57" t="n">
-        <v>0</v>
-      </c>
-      <c r="F57" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58">
@@ -1821,15 +1536,10 @@
       <c r="C58" t="n">
         <v>0</v>
       </c>
-      <c r="D58" t="inlineStr">
-        <is>
-          <t>CC[C@H]1OC(=O)[C@H](C)[C@@H](O[C@H]2C[C@@](C)(OC)[C@@H](O)[C@H](C)O2)[C@H](C)[C@@H](O[C@@H]2O[C@H](C)C[C@H](N(C)C)[C@H]2O)[C@](C)(O)C[C@@H](C)C(=O)[C@H](C)[C@@H](O)[C@]1(C)O</t>
-        </is>
+      <c r="D58" t="n">
+        <v>1</v>
       </c>
       <c r="E58" t="n">
-        <v>1</v>
-      </c>
-      <c r="F58" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1845,16 +1555,11 @@
       <c r="C59" t="n">
         <v>0</v>
       </c>
-      <c r="D59" t="inlineStr">
-        <is>
-          <t>O=C(O)Cc1ccccc1Nc1c(Cl)cccc1Cl</t>
-        </is>
+      <c r="D59" t="n">
+        <v>0</v>
       </c>
       <c r="E59" t="n">
         <v>1</v>
-      </c>
-      <c r="F59" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="60">
@@ -1869,16 +1574,11 @@
       <c r="C60" t="n">
         <v>0</v>
       </c>
-      <c r="D60" t="inlineStr">
-        <is>
-          <t>COc1ccnc(C[S+]([O-])c2nc3cc(OC(F)F)ccc3[nH]2)c1OC</t>
-        </is>
+      <c r="D60" t="n">
+        <v>0</v>
       </c>
       <c r="E60" t="n">
         <v>0</v>
-      </c>
-      <c r="F60" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="61">
@@ -1893,15 +1593,10 @@
       <c r="C61" t="n">
         <v>0</v>
       </c>
-      <c r="D61" t="inlineStr">
-        <is>
-          <t>CN(Cc1cc(Br)cc(Br)c1N)C1CCCCC1</t>
-        </is>
+      <c r="D61" t="n">
+        <v>0</v>
       </c>
       <c r="E61" t="n">
-        <v>0</v>
-      </c>
-      <c r="F61" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1917,15 +1612,10 @@
       <c r="C62" t="n">
         <v>0</v>
       </c>
-      <c r="D62" t="inlineStr">
-        <is>
-          <t>CC(=O)N1CCN(c2ccc(OCC3COC(Cn4ccnc4)(c4ccc(Cl)cc4Cl)O3)cc2)CC1</t>
-        </is>
+      <c r="D62" t="n">
+        <v>0</v>
       </c>
       <c r="E62" t="n">
-        <v>1</v>
-      </c>
-      <c r="F62" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1941,15 +1631,10 @@
       <c r="C63" t="n">
         <v>0</v>
       </c>
-      <c r="D63" t="inlineStr">
-        <is>
-          <t>CC[C@H]1OC(=O)[C@H](C)[C@@H](O[C@H]2C[C@@](C)(OC)[C@@H](O)[C@H](C)O2)[C@H](C)[C@@H](O[C@@H]2O[C@H](C)C[C@H](N(C)C)[C@H]2O)[C@](C)(OC)C[C@@H](C)C(=O)[C@H](C)[C@@H](O)[C@]1(C)O</t>
-        </is>
+      <c r="D63" t="n">
+        <v>1</v>
       </c>
       <c r="E63" t="n">
-        <v>0</v>
-      </c>
-      <c r="F63" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1965,15 +1650,10 @@
       <c r="C64" t="n">
         <v>0</v>
       </c>
-      <c r="D64" t="inlineStr">
-        <is>
-          <t>Nc1nc(=O)c2nc(CNc3ccc(C(=O)N[C@@H](CCC(=O)O)C(=O)O)cc3)cnc2[nH]1</t>
-        </is>
+      <c r="D64" t="n">
+        <v>0</v>
       </c>
       <c r="E64" t="n">
-        <v>0</v>
-      </c>
-      <c r="F64" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1989,16 +1669,11 @@
       <c r="C65" t="n">
         <v>0</v>
       </c>
-      <c r="D65" t="inlineStr">
-        <is>
-          <t>c1ccc2[nH]c(-c3cscn3)nc2c1</t>
-        </is>
+      <c r="D65" t="n">
+        <v>0</v>
       </c>
       <c r="E65" t="n">
         <v>1</v>
-      </c>
-      <c r="F65" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="66">
@@ -2013,15 +1688,10 @@
       <c r="C66" t="n">
         <v>0</v>
       </c>
-      <c r="D66" t="inlineStr">
-        <is>
-          <t>CCCCc1nc(Cl)c(CO)n1Cc1ccc(-c2ccccc2-c2nnn[nH]2)cc1</t>
-        </is>
+      <c r="D66" t="n">
+        <v>0</v>
       </c>
       <c r="E66" t="n">
-        <v>1</v>
-      </c>
-      <c r="F66" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2037,16 +1707,11 @@
       <c r="C67" t="n">
         <v>0</v>
       </c>
-      <c r="D67" t="inlineStr">
-        <is>
-          <t>CC(C)(C)NCC(O)c1ccc(O)c(CO)c1</t>
-        </is>
+      <c r="D67" t="n">
+        <v>0</v>
       </c>
       <c r="E67" t="n">
-        <v>0</v>
-      </c>
-      <c r="F67" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68">
@@ -2061,16 +1726,11 @@
       <c r="C68" t="n">
         <v>0</v>
       </c>
-      <c r="D68" t="inlineStr">
-        <is>
-          <t>C[C@H](CS)C(=O)N1CCC[C@H]1C(=O)O</t>
-        </is>
+      <c r="D68" t="n">
+        <v>0</v>
       </c>
       <c r="E68" t="n">
         <v>1</v>
-      </c>
-      <c r="F68" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="69">
@@ -2085,16 +1745,11 @@
       <c r="C69" t="n">
         <v>0</v>
       </c>
-      <c r="D69" t="inlineStr">
-        <is>
-          <t>CC(C)NCC(O)COc1cccc2ccccc12</t>
-        </is>
+      <c r="D69" t="n">
+        <v>0</v>
       </c>
       <c r="E69" t="n">
-        <v>0</v>
-      </c>
-      <c r="F69" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70">
@@ -2109,16 +1764,11 @@
       <c r="C70" t="n">
         <v>0</v>
       </c>
-      <c r="D70" t="inlineStr">
-        <is>
-          <t>Cn1c(=O)c2[nH]cnc2n(C)c1=O</t>
-        </is>
+      <c r="D70" t="n">
+        <v>0</v>
       </c>
       <c r="E70" t="n">
-        <v>0</v>
-      </c>
-      <c r="F70" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71">
@@ -2133,16 +1783,11 @@
       <c r="C71" t="n">
         <v>0</v>
       </c>
-      <c r="D71" t="inlineStr">
-        <is>
-          <t>O=C1O[C@H]([C@@H](O)CO)C(O)=C1O</t>
-        </is>
+      <c r="D71" t="n">
+        <v>0</v>
       </c>
       <c r="E71" t="n">
         <v>1</v>
-      </c>
-      <c r="F71" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="72">
@@ -2157,16 +1802,11 @@
       <c r="C72" t="n">
         <v>0</v>
       </c>
-      <c r="D72" t="inlineStr">
-        <is>
-          <t>CC1=C(/C=C/C(C)=C/C=C/C(C)=C\C(=O)O)C(C)(C)CCC1</t>
-        </is>
+      <c r="D72" t="n">
+        <v>0</v>
       </c>
       <c r="E72" t="n">
         <v>1</v>
-      </c>
-      <c r="F72" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="73">
@@ -2181,16 +1821,11 @@
       <c r="C73" t="n">
         <v>0</v>
       </c>
-      <c r="D73" t="inlineStr">
-        <is>
-          <t>O=C([O-])[C@H](O)[C@@H](O)[C@H](O)[C@H](O)CO.O=C([O-])[C@H](O)[C@@H](O)[C@H](O)[C@H](O)CO.[Zn+2]</t>
-        </is>
+      <c r="D73" t="n">
+        <v>0</v>
       </c>
       <c r="E73" t="n">
         <v>1</v>
-      </c>
-      <c r="F73" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="74">
@@ -2205,16 +1840,11 @@
       <c r="C74" t="n">
         <v>1</v>
       </c>
-      <c r="D74" t="inlineStr">
-        <is>
-          <t>CN(C)CCCOc1nn(Cc2ccccc2)c2ccccc12</t>
-        </is>
+      <c r="D74" t="n">
+        <v>0</v>
       </c>
       <c r="E74" t="n">
-        <v>0</v>
-      </c>
-      <c r="F74" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75">
@@ -2229,16 +1859,11 @@
       <c r="C75" t="n">
         <v>0</v>
       </c>
-      <c r="D75" t="inlineStr">
-        <is>
-          <t>OCCOCCN1CCN(C(c2ccccc2)c2ccc(Cl)cc2)CC1</t>
-        </is>
+      <c r="D75" t="n">
+        <v>0</v>
       </c>
       <c r="E75" t="n">
         <v>1</v>
-      </c>
-      <c r="F75" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="76">
@@ -2253,16 +1878,11 @@
       <c r="C76" t="n">
         <v>0</v>
       </c>
-      <c r="D76" t="inlineStr">
-        <is>
-          <t>COc1c(O[C@@H]2O[C@H](CO)[C@@H](O)[C@H](O)[C@H]2O)cc2c(c1OC)-c1ccc(SC)c(=O)cc1C(NC(C)=O)CC2</t>
-        </is>
+      <c r="D76" t="n">
+        <v>0</v>
       </c>
       <c r="E76" t="n">
         <v>1</v>
-      </c>
-      <c r="F76" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="77">
@@ -2277,16 +1897,11 @@
       <c r="C77" t="n">
         <v>0</v>
       </c>
-      <c r="D77" t="inlineStr">
-        <is>
-          <t>CC(C)NCC(O)c1ccc(NS(C)(=O)=O)cc1</t>
-        </is>
+      <c r="D77" t="n">
+        <v>0</v>
       </c>
       <c r="E77" t="n">
-        <v>0</v>
-      </c>
-      <c r="F77" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78">
@@ -2301,15 +1916,10 @@
       <c r="C78" t="n">
         <v>0</v>
       </c>
-      <c r="D78" t="inlineStr">
-        <is>
-          <t>COc1ccc(CCN(C)CCCC(C#N)(c2ccc(OC)c(OC)c2)C(C)C)cc1OC</t>
-        </is>
+      <c r="D78" t="n">
+        <v>1</v>
       </c>
       <c r="E78" t="n">
-        <v>0</v>
-      </c>
-      <c r="F78" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2325,15 +1935,10 @@
       <c r="C79" t="n">
         <v>0</v>
       </c>
-      <c r="D79" t="inlineStr">
-        <is>
-          <t>Nc1nc2c(ncn2COCCO)c(=O)[nH]1</t>
-        </is>
+      <c r="D79" t="n">
+        <v>0</v>
       </c>
       <c r="E79" t="n">
-        <v>0</v>
-      </c>
-      <c r="F79" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2349,15 +1954,10 @@
       <c r="C80" t="n">
         <v>0</v>
       </c>
-      <c r="D80" t="inlineStr">
-        <is>
-          <t>Cc1nccn1CC1CCc2c(c3ccccc3n2C)C1=O</t>
-        </is>
+      <c r="D80" t="n">
+        <v>0</v>
       </c>
       <c r="E80" t="n">
-        <v>1</v>
-      </c>
-      <c r="F80" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2373,16 +1973,11 @@
       <c r="C81" t="n">
         <v>0</v>
       </c>
-      <c r="D81" t="inlineStr">
-        <is>
-          <t>O=c1[nH]cc(F)c(=O)[nH]1</t>
-        </is>
+      <c r="D81" t="n">
+        <v>0</v>
       </c>
       <c r="E81" t="n">
         <v>1</v>
-      </c>
-      <c r="F81" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="82">
@@ -2397,15 +1992,10 @@
       <c r="C82" t="n">
         <v>0</v>
       </c>
-      <c r="D82" t="inlineStr">
-        <is>
-          <t>CCCc1nn(C)c2c(=O)[nH]c(-c3cc(S(=O)(=O)N4CCN(C)CC4)ccc3OCC)nc12</t>
-        </is>
+      <c r="D82" t="n">
+        <v>1</v>
       </c>
       <c r="E82" t="n">
-        <v>1</v>
-      </c>
-      <c r="F82" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2421,15 +2011,10 @@
       <c r="C83" t="n">
         <v>0</v>
       </c>
-      <c r="D83" t="inlineStr">
-        <is>
-          <t>CNCCC(Oc1ccc(C(F)(F)F)cc1)c1ccccc1</t>
-        </is>
+      <c r="D83" t="n">
+        <v>1</v>
       </c>
       <c r="E83" t="n">
-        <v>0</v>
-      </c>
-      <c r="F83" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2445,16 +2030,11 @@
       <c r="C84" t="n">
         <v>0</v>
       </c>
-      <c r="D84" t="inlineStr">
-        <is>
-          <t>CN[C@H]1CC[C@@H](c2ccc(Cl)c(Cl)c2)c2ccccc21</t>
-        </is>
+      <c r="D84" t="n">
+        <v>0</v>
       </c>
       <c r="E84" t="n">
         <v>1</v>
-      </c>
-      <c r="F84" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="85">
@@ -2469,16 +2049,11 @@
       <c r="C85" t="n">
         <v>0</v>
       </c>
-      <c r="D85" t="inlineStr">
-        <is>
-          <t>CN(C)CCCC1(c2ccc(F)cc2)OCc2cc(C#N)ccc21</t>
-        </is>
+      <c r="D85" t="n">
+        <v>1</v>
       </c>
       <c r="E85" t="n">
         <v>0</v>
-      </c>
-      <c r="F85" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="86">
@@ -2493,16 +2068,11 @@
       <c r="C86" t="n">
         <v>0</v>
       </c>
-      <c r="D86" t="inlineStr">
-        <is>
-          <t>CN(C)CCC[C@@]1(c2ccc(F)cc2)OCc2cc(C#N)ccc21</t>
-        </is>
+      <c r="D86" t="n">
+        <v>1</v>
       </c>
       <c r="E86" t="n">
         <v>0</v>
-      </c>
-      <c r="F86" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="87">
@@ -2517,16 +2087,11 @@
       <c r="C87" t="n">
         <v>0</v>
       </c>
-      <c r="D87" t="inlineStr">
-        <is>
-          <t>COc1ccc(C(CN(C)C)C2(O)CCCCC2)cc1</t>
-        </is>
+      <c r="D87" t="n">
+        <v>0</v>
       </c>
       <c r="E87" t="n">
-        <v>0</v>
-      </c>
-      <c r="F87" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="88">
@@ -2541,16 +2106,11 @@
       <c r="C88" t="n">
         <v>0</v>
       </c>
-      <c r="D88" t="inlineStr">
-        <is>
-          <t>CC(NC(C)(C)C)C(=O)c1cccc(Cl)c1</t>
-        </is>
+      <c r="D88" t="n">
+        <v>0</v>
       </c>
       <c r="E88" t="n">
         <v>1</v>
-      </c>
-      <c r="F88" t="n">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Replaced missing with mean v2
</commit_message>
<xml_diff>
--- a/outputs/clustered_examples.xlsx
+++ b/outputs/clustered_examples.xlsx
@@ -481,7 +481,7 @@
         <v>10.26</v>
       </c>
       <c r="E2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
         <v>1</v>
@@ -503,7 +503,7 @@
         <v>13.78</v>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
         <v>1</v>
@@ -525,7 +525,7 @@
         <v>13.07</v>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
         <v>1</v>
@@ -544,13 +544,13 @@
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>8.917755102040816</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
@@ -566,7 +566,7 @@
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>8.917755102040816</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
@@ -591,7 +591,7 @@
         <v>13.57</v>
       </c>
       <c r="E7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7" t="n">
         <v>1</v>
@@ -613,7 +613,7 @@
         <v>13.78</v>
       </c>
       <c r="E8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8" t="n">
         <v>1</v>
@@ -632,13 +632,13 @@
         <v>1</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>8.917755102040816</v>
       </c>
       <c r="E9" t="n">
         <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10">
@@ -654,7 +654,7 @@
         <v>1</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>8.917755102040816</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
@@ -679,7 +679,7 @@
         <v>13.8</v>
       </c>
       <c r="E11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F11" t="n">
         <v>1</v>
@@ -701,7 +701,7 @@
         <v>10.42</v>
       </c>
       <c r="E12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12" t="n">
         <v>1</v>
@@ -723,7 +723,7 @@
         <v>9.859999999999999</v>
       </c>
       <c r="E13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F13" t="n">
         <v>1</v>
@@ -745,7 +745,7 @@
         <v>10.39</v>
       </c>
       <c r="E14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F14" t="n">
         <v>1</v>
@@ -767,7 +767,7 @@
         <v>10.46</v>
       </c>
       <c r="E15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F15" t="n">
         <v>1</v>
@@ -789,10 +789,10 @@
         <v>10.28</v>
       </c>
       <c r="E16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F16" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17">
@@ -808,13 +808,13 @@
         <v>1</v>
       </c>
       <c r="D17" t="n">
-        <v>0</v>
+        <v>8.917755102040816</v>
       </c>
       <c r="E17" t="n">
         <v>0</v>
       </c>
       <c r="F17" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18">
@@ -830,13 +830,13 @@
         <v>1</v>
       </c>
       <c r="D18" t="n">
-        <v>0</v>
+        <v>8.917755102040816</v>
       </c>
       <c r="E18" t="n">
         <v>0</v>
       </c>
       <c r="F18" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19">
@@ -852,13 +852,13 @@
         <v>1</v>
       </c>
       <c r="D19" t="n">
-        <v>0</v>
+        <v>8.917755102040816</v>
       </c>
       <c r="E19" t="n">
         <v>0</v>
       </c>
       <c r="F19" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20">
@@ -874,13 +874,13 @@
         <v>1</v>
       </c>
       <c r="D20" t="n">
-        <v>0</v>
+        <v>8.917755102040816</v>
       </c>
       <c r="E20" t="n">
         <v>0</v>
       </c>
       <c r="F20" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21">
@@ -896,13 +896,13 @@
         <v>1</v>
       </c>
       <c r="D21" t="n">
-        <v>0</v>
+        <v>8.917755102040816</v>
       </c>
       <c r="E21" t="n">
         <v>0</v>
       </c>
       <c r="F21" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22">
@@ -921,7 +921,7 @@
         <v>13.96</v>
       </c>
       <c r="E22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F22" t="n">
         <v>1</v>
@@ -943,7 +943,7 @@
         <v>10.42</v>
       </c>
       <c r="E23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F23" t="n">
         <v>1</v>
@@ -965,7 +965,7 @@
         <v>10.07</v>
       </c>
       <c r="E24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F24" t="n">
         <v>1</v>
@@ -987,7 +987,7 @@
         <v>10.11</v>
       </c>
       <c r="E25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F25" t="n">
         <v>1</v>
@@ -1009,7 +1009,7 @@
         <v>10.11</v>
       </c>
       <c r="E26" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F26" t="n">
         <v>1</v>
@@ -1031,7 +1031,7 @@
         <v>10.07</v>
       </c>
       <c r="E27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F27" t="n">
         <v>1</v>
@@ -1050,13 +1050,13 @@
         <v>1</v>
       </c>
       <c r="D28" t="n">
-        <v>0</v>
+        <v>8.917755102040816</v>
       </c>
       <c r="E28" t="n">
         <v>0</v>
       </c>
       <c r="F28" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29">
@@ -1072,13 +1072,13 @@
         <v>0</v>
       </c>
       <c r="D29" t="n">
-        <v>0</v>
+        <v>8.917755102040816</v>
       </c>
       <c r="E29" t="n">
         <v>0</v>
       </c>
       <c r="F29" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30">
@@ -1097,7 +1097,7 @@
         <v>10.21</v>
       </c>
       <c r="E30" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F30" t="n">
         <v>1</v>
@@ -1116,13 +1116,13 @@
         <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>0</v>
+        <v>8.917755102040816</v>
       </c>
       <c r="E31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F31" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32">
@@ -1138,13 +1138,13 @@
         <v>0</v>
       </c>
       <c r="D32" t="n">
-        <v>0</v>
+        <v>8.917755102040816</v>
       </c>
       <c r="E32" t="n">
         <v>0</v>
       </c>
       <c r="F32" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
@@ -1163,10 +1163,10 @@
         <v>11.94</v>
       </c>
       <c r="E33" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F33" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34">
@@ -1182,7 +1182,7 @@
         <v>0</v>
       </c>
       <c r="D34" t="n">
-        <v>0</v>
+        <v>8.917755102040816</v>
       </c>
       <c r="E34" t="n">
         <v>0</v>
@@ -1207,7 +1207,7 @@
         <v>9.26</v>
       </c>
       <c r="E35" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F35" t="n">
         <v>1</v>
@@ -1226,7 +1226,7 @@
         <v>0</v>
       </c>
       <c r="D36" t="n">
-        <v>0</v>
+        <v>8.917755102040816</v>
       </c>
       <c r="E36" t="n">
         <v>0</v>
@@ -1254,7 +1254,7 @@
         <v>1</v>
       </c>
       <c r="F37" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38">
@@ -1273,10 +1273,10 @@
         <v>4.85</v>
       </c>
       <c r="E38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F38" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39">
@@ -1295,10 +1295,10 @@
         <v>3.41</v>
       </c>
       <c r="E39" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F39" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40">
@@ -1314,13 +1314,13 @@
         <v>0</v>
       </c>
       <c r="D40" t="n">
-        <v>0</v>
+        <v>8.917755102040816</v>
       </c>
       <c r="E40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F40" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41">
@@ -1336,13 +1336,13 @@
         <v>0</v>
       </c>
       <c r="D41" t="n">
-        <v>0</v>
+        <v>8.917755102040816</v>
       </c>
       <c r="E41" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F41" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="42">
@@ -1358,13 +1358,13 @@
         <v>0</v>
       </c>
       <c r="D42" t="n">
-        <v>0</v>
+        <v>8.917755102040816</v>
       </c>
       <c r="E42" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F42" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="43">
@@ -1380,13 +1380,13 @@
         <v>0</v>
       </c>
       <c r="D43" t="n">
-        <v>0</v>
+        <v>8.917755102040816</v>
       </c>
       <c r="E43" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F43" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="44">
@@ -1405,10 +1405,10 @@
         <v>12.43</v>
       </c>
       <c r="E44" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F44" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45">
@@ -1430,7 +1430,7 @@
         <v>1</v>
       </c>
       <c r="F45" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="46">
@@ -1446,13 +1446,13 @@
         <v>0</v>
       </c>
       <c r="D46" t="n">
-        <v>0</v>
+        <v>8.917755102040816</v>
       </c>
       <c r="E46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F46" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="47">
@@ -1468,13 +1468,13 @@
         <v>0</v>
       </c>
       <c r="D47" t="n">
-        <v>0</v>
+        <v>8.917755102040816</v>
       </c>
       <c r="E47" t="n">
         <v>0</v>
       </c>
       <c r="F47" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="48">
@@ -1493,10 +1493,10 @@
         <v>4.31</v>
       </c>
       <c r="E48" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F48" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="49">
@@ -1512,13 +1512,13 @@
         <v>0</v>
       </c>
       <c r="D49" t="n">
-        <v>0</v>
+        <v>8.917755102040816</v>
       </c>
       <c r="E49" t="n">
         <v>0</v>
       </c>
       <c r="F49" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="50">
@@ -1537,10 +1537,10 @@
         <v>4.25</v>
       </c>
       <c r="E50" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F50" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="51">
@@ -1559,10 +1559,10 @@
         <v>12.42</v>
       </c>
       <c r="E51" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F51" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="52">
@@ -1584,7 +1584,7 @@
         <v>1</v>
       </c>
       <c r="F52" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="53">
@@ -1600,13 +1600,13 @@
         <v>0</v>
       </c>
       <c r="D53" t="n">
-        <v>0</v>
+        <v>8.917755102040816</v>
       </c>
       <c r="E53" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F53" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="54">
@@ -1625,10 +1625,10 @@
         <v>0.27</v>
       </c>
       <c r="E54" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F54" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="55">
@@ -1650,7 +1650,7 @@
         <v>1</v>
       </c>
       <c r="F55" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="56">
@@ -1669,10 +1669,10 @@
         <v>4.32</v>
       </c>
       <c r="E56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F56" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="57">
@@ -1688,13 +1688,13 @@
         <v>0</v>
       </c>
       <c r="D57" t="n">
-        <v>0</v>
+        <v>8.917755102040816</v>
       </c>
       <c r="E57" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F57" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="58">
@@ -1713,10 +1713,10 @@
         <v>12.45</v>
       </c>
       <c r="E58" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F58" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59">
@@ -1735,10 +1735,10 @@
         <v>4</v>
       </c>
       <c r="E59" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F59" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="60">
@@ -1760,7 +1760,7 @@
         <v>1</v>
       </c>
       <c r="F60" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="61">
@@ -1776,13 +1776,13 @@
         <v>0</v>
       </c>
       <c r="D61" t="n">
-        <v>0</v>
+        <v>8.917755102040816</v>
       </c>
       <c r="E61" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F61" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="62">
@@ -1798,13 +1798,13 @@
         <v>0</v>
       </c>
       <c r="D62" t="n">
-        <v>0</v>
+        <v>8.917755102040816</v>
       </c>
       <c r="E62" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F62" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="63">
@@ -1823,10 +1823,10 @@
         <v>12.46</v>
       </c>
       <c r="E63" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F63" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64">
@@ -1845,10 +1845,10 @@
         <v>3.32</v>
       </c>
       <c r="E64" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F64" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="65">
@@ -1870,7 +1870,7 @@
         <v>1</v>
       </c>
       <c r="F65" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="66">
@@ -1889,10 +1889,10 @@
         <v>4.26</v>
       </c>
       <c r="E66" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F66" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="67">
@@ -1911,10 +1911,10 @@
         <v>10.12</v>
       </c>
       <c r="E67" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F67" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="68">
@@ -1933,10 +1933,10 @@
         <v>4.02</v>
       </c>
       <c r="E68" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F68" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="69">
@@ -1952,13 +1952,13 @@
         <v>0</v>
       </c>
       <c r="D69" t="n">
-        <v>0</v>
+        <v>8.917755102040816</v>
       </c>
       <c r="E69" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F69" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="70">
@@ -1980,7 +1980,7 @@
         <v>1</v>
       </c>
       <c r="F70" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="71">
@@ -1999,10 +1999,10 @@
         <v>4.36</v>
       </c>
       <c r="E71" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F71" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="72">
@@ -2024,7 +2024,7 @@
         <v>1</v>
       </c>
       <c r="F72" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="73">
@@ -2040,13 +2040,13 @@
         <v>0</v>
       </c>
       <c r="D73" t="n">
-        <v>0</v>
+        <v>8.917755102040816</v>
       </c>
       <c r="E73" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F73" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="74">
@@ -2062,13 +2062,13 @@
         <v>1</v>
       </c>
       <c r="D74" t="n">
-        <v>0</v>
+        <v>8.917755102040816</v>
       </c>
       <c r="E74" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F74" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="75">
@@ -2084,13 +2084,13 @@
         <v>0</v>
       </c>
       <c r="D75" t="n">
-        <v>0</v>
+        <v>8.917755102040816</v>
       </c>
       <c r="E75" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F75" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="76">
@@ -2109,10 +2109,10 @@
         <v>12.2</v>
       </c>
       <c r="E76" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F76" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="77">
@@ -2131,10 +2131,10 @@
         <v>10.07</v>
       </c>
       <c r="E77" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F77" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="78">
@@ -2150,13 +2150,13 @@
         <v>0</v>
       </c>
       <c r="D78" t="n">
-        <v>0</v>
+        <v>8.917755102040816</v>
       </c>
       <c r="E78" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F78" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="79">
@@ -2178,7 +2178,7 @@
         <v>1</v>
       </c>
       <c r="F79" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="80">
@@ -2194,13 +2194,13 @@
         <v>0</v>
       </c>
       <c r="D80" t="n">
-        <v>0</v>
+        <v>8.917755102040816</v>
       </c>
       <c r="E80" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F80" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="81">
@@ -2222,7 +2222,7 @@
         <v>1</v>
       </c>
       <c r="F81" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="82">
@@ -2244,7 +2244,7 @@
         <v>1</v>
       </c>
       <c r="F82" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="83">
@@ -2260,13 +2260,13 @@
         <v>0</v>
       </c>
       <c r="D83" t="n">
-        <v>0</v>
+        <v>8.917755102040816</v>
       </c>
       <c r="E83" t="n">
         <v>0</v>
       </c>
       <c r="F83" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="84">
@@ -2282,13 +2282,13 @@
         <v>0</v>
       </c>
       <c r="D84" t="n">
-        <v>0</v>
+        <v>8.917755102040816</v>
       </c>
       <c r="E84" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F84" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="85">
@@ -2304,13 +2304,13 @@
         <v>0</v>
       </c>
       <c r="D85" t="n">
-        <v>0</v>
+        <v>8.917755102040816</v>
       </c>
       <c r="E85" t="n">
         <v>0</v>
       </c>
       <c r="F85" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="86">
@@ -2326,13 +2326,13 @@
         <v>0</v>
       </c>
       <c r="D86" t="n">
-        <v>0</v>
+        <v>8.917755102040816</v>
       </c>
       <c r="E86" t="n">
         <v>0</v>
       </c>
       <c r="F86" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87">
@@ -2348,13 +2348,13 @@
         <v>0</v>
       </c>
       <c r="D87" t="n">
-        <v>0</v>
+        <v>8.917755102040816</v>
       </c>
       <c r="E87" t="n">
         <v>0</v>
       </c>
       <c r="F87" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="88">
@@ -2370,13 +2370,13 @@
         <v>0</v>
       </c>
       <c r="D88" t="n">
-        <v>0</v>
+        <v>8.917755102040816</v>
       </c>
       <c r="E88" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F88" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added dbscan with no tsne
</commit_message>
<xml_diff>
--- a/outputs/clustered_examples.xlsx
+++ b/outputs/clustered_examples.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F88"/>
+  <dimension ref="A1:G88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,10 +456,15 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>km_cluster</t>
+          <t>tsne_km_cluster</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>tsne_db_cluster</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>db_cluster</t>
         </is>
@@ -486,6 +491,9 @@
       <c r="F2" t="n">
         <v>0</v>
       </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -508,6 +516,9 @@
       <c r="F3" t="n">
         <v>0</v>
       </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -530,6 +541,9 @@
       <c r="F4" t="n">
         <v>0</v>
       </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -552,6 +566,9 @@
       <c r="F5" t="n">
         <v>0</v>
       </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -574,6 +591,9 @@
       <c r="F6" t="n">
         <v>0</v>
       </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -596,6 +616,9 @@
       <c r="F7" t="n">
         <v>0</v>
       </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -618,6 +641,9 @@
       <c r="F8" t="n">
         <v>0</v>
       </c>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -635,9 +661,12 @@
         <v>8.917755102040816</v>
       </c>
       <c r="E9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" t="n">
         <v>0</v>
       </c>
     </row>
@@ -662,6 +691,9 @@
       <c r="F10" t="n">
         <v>0</v>
       </c>
+      <c r="G10" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -684,6 +716,9 @@
       <c r="F11" t="n">
         <v>0</v>
       </c>
+      <c r="G11" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
@@ -706,6 +741,9 @@
       <c r="F12" t="n">
         <v>0</v>
       </c>
+      <c r="G12" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
@@ -728,6 +766,9 @@
       <c r="F13" t="n">
         <v>0</v>
       </c>
+      <c r="G13" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
@@ -748,6 +789,9 @@
         <v>1</v>
       </c>
       <c r="F14" t="n">
+        <v>1</v>
+      </c>
+      <c r="G14" t="n">
         <v>0</v>
       </c>
     </row>
@@ -772,6 +816,9 @@
       <c r="F15" t="n">
         <v>0</v>
       </c>
+      <c r="G15" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
@@ -789,9 +836,12 @@
         <v>10.28</v>
       </c>
       <c r="E16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" t="n">
         <v>0</v>
       </c>
     </row>
@@ -811,9 +861,12 @@
         <v>8.917755102040816</v>
       </c>
       <c r="E17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F17" t="n">
+        <v>0</v>
+      </c>
+      <c r="G17" t="n">
         <v>0</v>
       </c>
     </row>
@@ -833,9 +886,12 @@
         <v>8.917755102040816</v>
       </c>
       <c r="E18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F18" t="n">
+        <v>0</v>
+      </c>
+      <c r="G18" t="n">
         <v>0</v>
       </c>
     </row>
@@ -855,9 +911,12 @@
         <v>8.917755102040816</v>
       </c>
       <c r="E19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F19" t="n">
+        <v>0</v>
+      </c>
+      <c r="G19" t="n">
         <v>0</v>
       </c>
     </row>
@@ -877,9 +936,12 @@
         <v>8.917755102040816</v>
       </c>
       <c r="E20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F20" t="n">
+        <v>0</v>
+      </c>
+      <c r="G20" t="n">
         <v>0</v>
       </c>
     </row>
@@ -899,9 +961,12 @@
         <v>8.917755102040816</v>
       </c>
       <c r="E21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F21" t="n">
+        <v>0</v>
+      </c>
+      <c r="G21" t="n">
         <v>0</v>
       </c>
     </row>
@@ -926,6 +991,9 @@
       <c r="F22" t="n">
         <v>0</v>
       </c>
+      <c r="G22" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
@@ -948,6 +1016,9 @@
       <c r="F23" t="n">
         <v>0</v>
       </c>
+      <c r="G23" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
@@ -968,6 +1039,9 @@
         <v>1</v>
       </c>
       <c r="F24" t="n">
+        <v>1</v>
+      </c>
+      <c r="G24" t="n">
         <v>0</v>
       </c>
     </row>
@@ -992,6 +1066,9 @@
       <c r="F25" t="n">
         <v>0</v>
       </c>
+      <c r="G25" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
@@ -1012,6 +1089,9 @@
         <v>1</v>
       </c>
       <c r="F26" t="n">
+        <v>1</v>
+      </c>
+      <c r="G26" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1034,6 +1114,9 @@
         <v>1</v>
       </c>
       <c r="F27" t="n">
+        <v>1</v>
+      </c>
+      <c r="G27" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1053,9 +1136,12 @@
         <v>8.917755102040816</v>
       </c>
       <c r="E28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F28" t="n">
+        <v>0</v>
+      </c>
+      <c r="G28" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1075,9 +1161,12 @@
         <v>8.917755102040816</v>
       </c>
       <c r="E29" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F29" t="n">
+        <v>0</v>
+      </c>
+      <c r="G29" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1102,6 +1191,9 @@
       <c r="F30" t="n">
         <v>0</v>
       </c>
+      <c r="G30" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
@@ -1124,6 +1216,9 @@
       <c r="F31" t="n">
         <v>0</v>
       </c>
+      <c r="G31" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
@@ -1146,6 +1241,9 @@
       <c r="F32" t="n">
         <v>0</v>
       </c>
+      <c r="G32" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
@@ -1168,6 +1266,9 @@
       <c r="F33" t="n">
         <v>0</v>
       </c>
+      <c r="G33" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
@@ -1190,6 +1291,9 @@
       <c r="F34" t="n">
         <v>0</v>
       </c>
+      <c r="G34" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
@@ -1212,6 +1316,9 @@
       <c r="F35" t="n">
         <v>0</v>
       </c>
+      <c r="G35" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
@@ -1234,6 +1341,9 @@
       <c r="F36" t="n">
         <v>0</v>
       </c>
+      <c r="G36" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
@@ -1256,6 +1366,9 @@
       <c r="F37" t="n">
         <v>0</v>
       </c>
+      <c r="G37" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
@@ -1276,6 +1389,9 @@
         <v>0</v>
       </c>
       <c r="F38" t="n">
+        <v>2</v>
+      </c>
+      <c r="G38" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1298,6 +1414,9 @@
         <v>0</v>
       </c>
       <c r="F39" t="n">
+        <v>2</v>
+      </c>
+      <c r="G39" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1322,6 +1441,9 @@
       <c r="F40" t="n">
         <v>0</v>
       </c>
+      <c r="G40" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
@@ -1344,6 +1466,9 @@
       <c r="F41" t="n">
         <v>0</v>
       </c>
+      <c r="G41" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="inlineStr">
@@ -1366,6 +1491,9 @@
       <c r="F42" t="n">
         <v>0</v>
       </c>
+      <c r="G42" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="inlineStr">
@@ -1388,6 +1516,9 @@
       <c r="F43" t="n">
         <v>0</v>
       </c>
+      <c r="G43" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
@@ -1410,6 +1541,9 @@
       <c r="F44" t="n">
         <v>0</v>
       </c>
+      <c r="G44" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="inlineStr">
@@ -1430,6 +1564,9 @@
         <v>0</v>
       </c>
       <c r="F45" t="n">
+        <v>2</v>
+      </c>
+      <c r="G45" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1454,6 +1591,9 @@
       <c r="F46" t="n">
         <v>0</v>
       </c>
+      <c r="G46" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="inlineStr">
@@ -1476,6 +1616,9 @@
       <c r="F47" t="n">
         <v>0</v>
       </c>
+      <c r="G47" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="inlineStr">
@@ -1498,6 +1641,9 @@
       <c r="F48" t="n">
         <v>0</v>
       </c>
+      <c r="G48" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="inlineStr">
@@ -1520,6 +1666,9 @@
       <c r="F49" t="n">
         <v>0</v>
       </c>
+      <c r="G49" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="inlineStr">
@@ -1542,6 +1691,9 @@
       <c r="F50" t="n">
         <v>0</v>
       </c>
+      <c r="G50" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="inlineStr">
@@ -1564,6 +1716,9 @@
       <c r="F51" t="n">
         <v>0</v>
       </c>
+      <c r="G51" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="inlineStr">
@@ -1586,6 +1741,9 @@
       <c r="F52" t="n">
         <v>0</v>
       </c>
+      <c r="G52" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="inlineStr">
@@ -1608,6 +1766,9 @@
       <c r="F53" t="n">
         <v>0</v>
       </c>
+      <c r="G53" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="inlineStr">
@@ -1630,6 +1791,9 @@
       <c r="F54" t="n">
         <v>0</v>
       </c>
+      <c r="G54" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="inlineStr">
@@ -1652,6 +1816,9 @@
       <c r="F55" t="n">
         <v>0</v>
       </c>
+      <c r="G55" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="inlineStr">
@@ -1674,6 +1841,9 @@
       <c r="F56" t="n">
         <v>0</v>
       </c>
+      <c r="G56" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="inlineStr">
@@ -1696,6 +1866,9 @@
       <c r="F57" t="n">
         <v>0</v>
       </c>
+      <c r="G57" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="inlineStr">
@@ -1718,6 +1891,9 @@
       <c r="F58" t="n">
         <v>0</v>
       </c>
+      <c r="G58" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="inlineStr">
@@ -1740,6 +1916,9 @@
       <c r="F59" t="n">
         <v>0</v>
       </c>
+      <c r="G59" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="inlineStr">
@@ -1762,6 +1941,9 @@
       <c r="F60" t="n">
         <v>0</v>
       </c>
+      <c r="G60" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="inlineStr">
@@ -1779,9 +1961,12 @@
         <v>8.917755102040816</v>
       </c>
       <c r="E61" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F61" t="n">
+        <v>0</v>
+      </c>
+      <c r="G61" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1806,6 +1991,9 @@
       <c r="F62" t="n">
         <v>0</v>
       </c>
+      <c r="G62" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="inlineStr">
@@ -1828,6 +2016,9 @@
       <c r="F63" t="n">
         <v>0</v>
       </c>
+      <c r="G63" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="inlineStr">
@@ -1850,6 +2041,9 @@
       <c r="F64" t="n">
         <v>0</v>
       </c>
+      <c r="G64" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="inlineStr">
@@ -1872,6 +2066,9 @@
       <c r="F65" t="n">
         <v>0</v>
       </c>
+      <c r="G65" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="inlineStr">
@@ -1894,6 +2091,9 @@
       <c r="F66" t="n">
         <v>0</v>
       </c>
+      <c r="G66" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="inlineStr">
@@ -1911,9 +2111,12 @@
         <v>10.12</v>
       </c>
       <c r="E67" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F67" t="n">
+        <v>0</v>
+      </c>
+      <c r="G67" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1936,6 +2139,9 @@
         <v>0</v>
       </c>
       <c r="F68" t="n">
+        <v>2</v>
+      </c>
+      <c r="G68" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1960,6 +2166,9 @@
       <c r="F69" t="n">
         <v>0</v>
       </c>
+      <c r="G69" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="inlineStr">
@@ -1982,6 +2191,9 @@
       <c r="F70" t="n">
         <v>0</v>
       </c>
+      <c r="G70" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="inlineStr">
@@ -2002,6 +2214,9 @@
         <v>0</v>
       </c>
       <c r="F71" t="n">
+        <v>2</v>
+      </c>
+      <c r="G71" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2026,6 +2241,9 @@
       <c r="F72" t="n">
         <v>0</v>
       </c>
+      <c r="G72" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="inlineStr">
@@ -2048,6 +2266,9 @@
       <c r="F73" t="n">
         <v>0</v>
       </c>
+      <c r="G73" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="inlineStr">
@@ -2065,9 +2286,12 @@
         <v>8.917755102040816</v>
       </c>
       <c r="E74" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F74" t="n">
+        <v>0</v>
+      </c>
+      <c r="G74" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2092,6 +2316,9 @@
       <c r="F75" t="n">
         <v>0</v>
       </c>
+      <c r="G75" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="inlineStr">
@@ -2114,6 +2341,9 @@
       <c r="F76" t="n">
         <v>0</v>
       </c>
+      <c r="G76" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="inlineStr">
@@ -2136,6 +2366,9 @@
       <c r="F77" t="n">
         <v>0</v>
       </c>
+      <c r="G77" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="inlineStr">
@@ -2158,6 +2391,9 @@
       <c r="F78" t="n">
         <v>0</v>
       </c>
+      <c r="G78" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="inlineStr">
@@ -2180,6 +2416,9 @@
       <c r="F79" t="n">
         <v>0</v>
       </c>
+      <c r="G79" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="inlineStr">
@@ -2202,6 +2441,9 @@
       <c r="F80" t="n">
         <v>0</v>
       </c>
+      <c r="G80" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="inlineStr">
@@ -2224,6 +2466,9 @@
       <c r="F81" t="n">
         <v>0</v>
       </c>
+      <c r="G81" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="inlineStr">
@@ -2246,6 +2491,9 @@
       <c r="F82" t="n">
         <v>0</v>
       </c>
+      <c r="G82" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="inlineStr">
@@ -2263,9 +2511,12 @@
         <v>8.917755102040816</v>
       </c>
       <c r="E83" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F83" t="n">
+        <v>0</v>
+      </c>
+      <c r="G83" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2290,6 +2541,9 @@
       <c r="F84" t="n">
         <v>0</v>
       </c>
+      <c r="G84" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="inlineStr">
@@ -2307,9 +2561,12 @@
         <v>8.917755102040816</v>
       </c>
       <c r="E85" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F85" t="n">
+        <v>0</v>
+      </c>
+      <c r="G85" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2329,9 +2586,12 @@
         <v>8.917755102040816</v>
       </c>
       <c r="E86" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F86" t="n">
+        <v>0</v>
+      </c>
+      <c r="G86" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2351,9 +2611,12 @@
         <v>8.917755102040816</v>
       </c>
       <c r="E87" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F87" t="n">
+        <v>0</v>
+      </c>
+      <c r="G87" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2376,6 +2639,9 @@
         <v>0</v>
       </c>
       <c r="F88" t="n">
+        <v>0</v>
+      </c>
+      <c r="G88" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>